<commit_message>
Sauvegarde locale avant rebase
</commit_message>
<xml_diff>
--- a/factures_comptables_nettoyees.xlsx
+++ b/factures_comptables_nettoyees.xlsx
@@ -37,19 +37,19 @@
     <t>solde_cumulé</t>
   </si>
   <si>
-    <t>601.0</t>
-  </si>
-  <si>
-    <t>44566.0</t>
-  </si>
-  <si>
-    <t>512.0</t>
-  </si>
-  <si>
-    <t>411.0</t>
-  </si>
-  <si>
-    <t>606.0</t>
+    <t>601</t>
+  </si>
+  <si>
+    <t>44566</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>411</t>
+  </si>
+  <si>
+    <t>606</t>
   </si>
   <si>
     <t>Achat de matières premières</t>

</xml_diff>